<commit_message>
Borg results, first visualizations
</commit_message>
<xml_diff>
--- a/Borg/progress.xlsx
+++ b/Borg/progress.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emma\PythonProjects\thesis2\thesis\Borg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503184CC-D32A-4095-A536-FA47659ADEE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B867A5-AF0E-4E5E-BEB7-C268C6B22F8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E205B068-EFB7-46BC-9393-E3B234ED48FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Blad1!$B$1:$B$90</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$1:$B$90</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -157,7 +153,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.0888340118136482E-2"/>
+          <c:y val="7.9510484877371529E-2"/>
+          <c:w val="0.95251026051370291"/>
+          <c:h val="0.88641805367448323"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -459,6 +465,889 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-601E-486C-8CEA-52257F6B5CBE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Blad1!$E$1:$E$284</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="284"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>616</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>633</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>726</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>737</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>755</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>769</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>856</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>864</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>882</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>885</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>892</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>895</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>902</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>922</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>929</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>937</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>942</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>946</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>958</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>964</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>969</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>972</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>974</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>977</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>984</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>988</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>993</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1012</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1023</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1037</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1098</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1102</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1104</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1106</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1114</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1117</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1130</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1133</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1145</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1154</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1156</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1159</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1162</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1165</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1172</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1175</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1178</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1184</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1188</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1192</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1192</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1199</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1203</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1207</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1210</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1217</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1228</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1233</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1238</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1241</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1243</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1247</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1248</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1253</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1257</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1262</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1268</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1269</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1274</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1278</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1283</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1284</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1286</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1288</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1291</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1294</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1297</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1301</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1302</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1305</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1308</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1311</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1314</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1316</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1319</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1322</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1326</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1329</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1334</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1336</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1337</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1344</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1347</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1351</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1359</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1362</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1364</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1365</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1376</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1379</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1383</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1384</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1389</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1393</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1396</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1399</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1404</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1412</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1413</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1413</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1415</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1422</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1424</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1426</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1430</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1433</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1436</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1437</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1437</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1439</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1439</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1443</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1445</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1453</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1455</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1457</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1459</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1460</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1464</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1465</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1466</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1475</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1478</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1481</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1482</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1484</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1492</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1495</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1498</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1503</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1506</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1509</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>1509</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1511</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1513</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1559</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1561</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1562</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1562</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1565</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1571</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1576</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1578</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1581</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1583</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1584</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1586</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1589</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1591</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1596</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1597</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1599</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1601</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1603</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1605</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1606</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1609</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1611</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1613</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1615</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1618</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1622</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1624</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1627</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1631</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1639</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1639</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1642</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1645</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1648</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1652</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1658</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1660</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1661</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>1662</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>1662</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1664</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>1665</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>1666</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>1670</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>1674</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>1676</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7072-45FC-B30A-CF2918E4DA3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -633,10 +1522,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1189,16 +2081,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1523,576 +2415,3821 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FAFA1D6-39AB-4B4B-B2B7-8BBB51961004}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:G284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N276" sqref="N276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>100</v>
+      </c>
+      <c r="E1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>201</v>
+      </c>
+      <c r="E2">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <f>E2-E1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>341</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">E3-E2</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>442</v>
+      </c>
+      <c r="E4">
+        <v>128</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>210</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>850</v>
+      </c>
+      <c r="E5">
+        <v>226</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>291</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>950</v>
+      </c>
+      <c r="E6">
+        <v>247</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>313</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1494</v>
+      </c>
+      <c r="E7">
+        <v>321</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>410</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1594</v>
+      </c>
+      <c r="E8">
+        <v>331</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>422</v>
       </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1694</v>
+      </c>
+      <c r="E9">
+        <v>345</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>536</v>
       </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1794</v>
+      </c>
+      <c r="E10">
+        <v>354</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>549</v>
       </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2510</v>
+      </c>
+      <c r="E11">
+        <v>433</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>562</v>
       </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>2610</v>
+      </c>
+      <c r="E12">
+        <v>440</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>576</v>
       </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>2710</v>
+      </c>
+      <c r="E13">
+        <v>451</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>586</v>
       </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>2810</v>
+      </c>
+      <c r="E14">
+        <v>462</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>596</v>
       </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2910</v>
+      </c>
+      <c r="E15">
+        <v>469</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>607</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3011</v>
+      </c>
+      <c r="E16">
+        <v>477</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>618</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>3112</v>
+      </c>
+      <c r="E17">
+        <v>487</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>624</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>3213</v>
+      </c>
+      <c r="E18">
+        <v>495</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>630</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3313</v>
+      </c>
+      <c r="E19">
+        <v>505</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>638</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>3414</v>
+      </c>
+      <c r="E20">
+        <v>516</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>644</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>4346</v>
+      </c>
+      <c r="E21">
+        <v>590</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>657</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>4447</v>
+      </c>
+      <c r="E22">
+        <v>596</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>663</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>4547</v>
+      </c>
+      <c r="E23">
+        <v>603</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>670</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>4647</v>
+      </c>
+      <c r="E24">
+        <v>616</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>677</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>4747</v>
+      </c>
+      <c r="E25">
+        <v>624</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>740</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>4848</v>
+      </c>
+      <c r="E26">
+        <v>633</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>752</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>4949</v>
+      </c>
+      <c r="E27">
+        <v>640</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>763</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>5049</v>
+      </c>
+      <c r="E28">
+        <v>649</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>770</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>5149</v>
+      </c>
+      <c r="E29">
+        <v>660</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>778</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>5249</v>
+      </c>
+      <c r="E30">
+        <v>665</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>791</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>5350</v>
+      </c>
+      <c r="E31">
+        <v>670</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>799</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5450</v>
+      </c>
+      <c r="E32">
+        <v>679</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>809</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>5550</v>
+      </c>
+      <c r="E33">
+        <v>686</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>813</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>5650</v>
+      </c>
+      <c r="E34">
+        <v>696</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>820</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>5750</v>
+      </c>
+      <c r="E35">
+        <v>705</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>827</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>5851</v>
+      </c>
+      <c r="E36">
+        <v>714</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>834</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5951</v>
+      </c>
+      <c r="E37">
+        <v>722</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>841</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>6052</v>
+      </c>
+      <c r="E38">
+        <v>726</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>856</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>6152</v>
+      </c>
+      <c r="E39">
+        <v>732</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>863</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>6252</v>
+      </c>
+      <c r="E40">
+        <v>737</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>937</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>6353</v>
+      </c>
+      <c r="E41">
+        <v>741</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>944</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>6453</v>
+      </c>
+      <c r="E42">
+        <v>746</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>950</v>
       </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>6553</v>
+      </c>
+      <c r="E43">
+        <v>755</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>954</v>
       </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>6653</v>
+      </c>
+      <c r="E44">
+        <v>760</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>965</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>6754</v>
+      </c>
+      <c r="E45">
+        <v>769</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>974</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>6854</v>
+      </c>
+      <c r="E46">
+        <v>773</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>982</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>6954</v>
+      </c>
+      <c r="E47">
+        <v>776</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>987</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>7055</v>
+      </c>
+      <c r="E48">
+        <v>780</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>993</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>7155</v>
+      </c>
+      <c r="E49">
+        <v>784</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>1001</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>7256</v>
+      </c>
+      <c r="E50">
+        <v>790</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <f>SUM(F22:F50)/29</f>
+        <v>6.8965517241379306</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>1006</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>8481</v>
+      </c>
+      <c r="E51">
+        <v>855</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>1011</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>8582</v>
+      </c>
+      <c r="E52">
+        <v>856</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>1017</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>8682</v>
+      </c>
+      <c r="E53">
+        <v>864</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8972</v>
       </c>
       <c r="B54">
         <v>1033</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>8783</v>
+      </c>
+      <c r="E54">
+        <v>870</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9072</v>
       </c>
       <c r="B55">
         <v>1039</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>8884</v>
+      </c>
+      <c r="E55">
+        <v>875</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9172</v>
       </c>
       <c r="B56">
         <v>1044</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>8985</v>
+      </c>
+      <c r="E56">
+        <v>882</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9272</v>
       </c>
       <c r="B57">
         <v>1051</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>9086</v>
+      </c>
+      <c r="E57">
+        <v>885</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9373</v>
       </c>
       <c r="B58">
         <v>1058</v>
       </c>
-      <c r="C58">
-        <v>9373</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>9187</v>
+      </c>
+      <c r="E58">
+        <v>892</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9473</v>
       </c>
       <c r="B59">
         <v>1069</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>9287</v>
+      </c>
+      <c r="E59">
+        <v>895</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9674</v>
       </c>
       <c r="B60">
         <v>1089</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>9388</v>
+      </c>
+      <c r="E60">
+        <v>902</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9775</v>
       </c>
       <c r="B61">
         <v>1091</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>9488</v>
+      </c>
+      <c r="E61">
+        <v>908</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9875</v>
       </c>
       <c r="B62">
         <v>1098</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>9588</v>
+      </c>
+      <c r="E62">
+        <v>915</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9975</v>
       </c>
       <c r="B63">
         <v>1108</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>9689</v>
+      </c>
+      <c r="E63">
+        <v>918</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>10076</v>
       </c>
       <c r="B64">
         <v>1116</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>9789</v>
+      </c>
+      <c r="E64">
+        <v>922</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>10177</v>
       </c>
       <c r="B65">
         <v>1121</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>9889</v>
+      </c>
+      <c r="E65">
+        <v>925</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>10278</v>
       </c>
       <c r="B66">
         <v>1128</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>9990</v>
+      </c>
+      <c r="E66">
+        <v>929</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>10379</v>
       </c>
       <c r="B67">
         <v>1136</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>10091</v>
+      </c>
+      <c r="E67">
+        <v>937</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="1">E67-E66</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>12173</v>
       </c>
       <c r="B68">
         <v>1217</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>10191</v>
+      </c>
+      <c r="E68">
+        <v>942</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>12273</v>
       </c>
       <c r="B69">
         <v>1223</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>10292</v>
+      </c>
+      <c r="E69">
+        <v>946</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>12373</v>
       </c>
       <c r="B70">
         <v>1233</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>10393</v>
+      </c>
+      <c r="E70">
+        <v>951</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>12474</v>
       </c>
       <c r="B71">
         <v>1238</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>10493</v>
+      </c>
+      <c r="E71">
+        <v>958</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>12575</v>
       </c>
       <c r="B72">
         <v>1245</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>10593</v>
+      </c>
+      <c r="E72">
+        <v>964</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>12676</v>
       </c>
       <c r="B73">
         <v>1250</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>10693</v>
+      </c>
+      <c r="E73">
+        <v>969</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>12777</v>
       </c>
       <c r="B74">
         <v>1256</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>10793</v>
+      </c>
+      <c r="E74">
+        <v>972</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>12878</v>
       </c>
       <c r="B75">
         <v>1267</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>10894</v>
+      </c>
+      <c r="E75">
+        <v>974</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>12979</v>
       </c>
       <c r="B76">
         <v>1276</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>10994</v>
+      </c>
+      <c r="E76">
+        <v>977</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>13079</v>
       </c>
       <c r="B77">
         <v>1286</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>11094</v>
+      </c>
+      <c r="E77">
+        <v>980</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>13179</v>
       </c>
       <c r="B78">
         <v>1289</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>11195</v>
+      </c>
+      <c r="E78">
+        <v>984</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>13279</v>
       </c>
       <c r="B79">
         <v>1295</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>11295</v>
+      </c>
+      <c r="E79">
+        <v>988</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>13380</v>
       </c>
       <c r="B80">
         <v>1300</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>11395</v>
+      </c>
+      <c r="E80">
+        <v>993</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>13480</v>
       </c>
       <c r="B81">
         <v>1306</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>11495</v>
+      </c>
+      <c r="E81">
+        <v>1000</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>13580</v>
       </c>
       <c r="B82">
         <v>1310</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>11595</v>
+      </c>
+      <c r="E82">
+        <v>1005</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>13680</v>
       </c>
       <c r="B83">
         <v>1316</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>11695</v>
+      </c>
+      <c r="E83">
+        <v>1009</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>13780</v>
       </c>
       <c r="B84">
         <v>1320</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>11796</v>
+      </c>
+      <c r="E84">
+        <v>1012</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>13881</v>
       </c>
       <c r="B85">
         <v>1325</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>11896</v>
+      </c>
+      <c r="E85">
+        <v>1017</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>13982</v>
       </c>
       <c r="B86">
         <v>1330</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>11996</v>
+      </c>
+      <c r="E86">
+        <v>1023</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>14082</v>
       </c>
       <c r="B87">
         <v>1337</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>12096</v>
+      </c>
+      <c r="E87">
+        <v>1030</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>14183</v>
       </c>
       <c r="B88">
         <v>1341</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>12196</v>
+      </c>
+      <c r="E88">
+        <v>1037</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G88">
+        <f>SUM(F52:F88)/37</f>
+        <v>4.9189189189189193</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>14284</v>
       </c>
       <c r="B89">
         <v>1352</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>13801</v>
+      </c>
+      <c r="E89">
+        <v>1098</v>
+      </c>
+      <c r="F89">
+        <f>E89-E88</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>14385</v>
       </c>
       <c r="B90">
         <v>1356</v>
+      </c>
+      <c r="D90">
+        <v>13901</v>
+      </c>
+      <c r="E90">
+        <v>1102</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>14002</v>
+      </c>
+      <c r="E91">
+        <v>1104</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>14102</v>
+      </c>
+      <c r="E92">
+        <v>1106</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>14202</v>
+      </c>
+      <c r="E93">
+        <v>1110</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>14302</v>
+      </c>
+      <c r="E94">
+        <v>1114</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>14403</v>
+      </c>
+      <c r="E95">
+        <v>1117</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>14503</v>
+      </c>
+      <c r="E96">
+        <v>1122</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>14603</v>
+      </c>
+      <c r="E97">
+        <v>1130</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>14704</v>
+      </c>
+      <c r="E98">
+        <v>1133</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>14805</v>
+      </c>
+      <c r="E99">
+        <v>1140</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>14905</v>
+      </c>
+      <c r="E100">
+        <v>1145</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>15005</v>
+      </c>
+      <c r="E101">
+        <v>1148</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>15106</v>
+      </c>
+      <c r="E102">
+        <v>1150</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>15206</v>
+      </c>
+      <c r="E103">
+        <v>1154</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>15307</v>
+      </c>
+      <c r="E104">
+        <v>1156</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>15407</v>
+      </c>
+      <c r="E105">
+        <v>1159</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>15507</v>
+      </c>
+      <c r="E106">
+        <v>1162</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>15607</v>
+      </c>
+      <c r="E107">
+        <v>1165</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>15707</v>
+      </c>
+      <c r="E108">
+        <v>1172</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>15808</v>
+      </c>
+      <c r="E109">
+        <v>1175</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>15909</v>
+      </c>
+      <c r="E110">
+        <v>1178</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>16009</v>
+      </c>
+      <c r="E111">
+        <v>1184</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>16110</v>
+      </c>
+      <c r="E112">
+        <v>1188</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>16211</v>
+      </c>
+      <c r="E113">
+        <v>1192</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>16311</v>
+      </c>
+      <c r="E114">
+        <v>1192</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>16412</v>
+      </c>
+      <c r="E115">
+        <v>1197</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>16513</v>
+      </c>
+      <c r="E116">
+        <v>1199</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>16613</v>
+      </c>
+      <c r="E117">
+        <v>1203</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>16713</v>
+      </c>
+      <c r="E118">
+        <v>1207</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>16813</v>
+      </c>
+      <c r="E119">
+        <v>1210</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>16914</v>
+      </c>
+      <c r="E120">
+        <v>1215</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>17015</v>
+      </c>
+      <c r="E121">
+        <v>1217</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>17116</v>
+      </c>
+      <c r="E122">
+        <v>1225</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>17216</v>
+      </c>
+      <c r="E123">
+        <v>1228</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>17316</v>
+      </c>
+      <c r="E124">
+        <v>1233</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>17416</v>
+      </c>
+      <c r="E125">
+        <v>1238</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>17517</v>
+      </c>
+      <c r="E126">
+        <v>1241</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>17617</v>
+      </c>
+      <c r="E127">
+        <v>1243</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>17717</v>
+      </c>
+      <c r="E128">
+        <v>1247</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>17817</v>
+      </c>
+      <c r="E129">
+        <v>1248</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>17917</v>
+      </c>
+      <c r="E130">
+        <v>1253</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>18017</v>
+      </c>
+      <c r="E131">
+        <v>1257</v>
+      </c>
+      <c r="F131">
+        <f t="shared" ref="F131:F194" si="2">E131-E130</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <v>18117</v>
+      </c>
+      <c r="E132">
+        <v>1262</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <v>18217</v>
+      </c>
+      <c r="E133">
+        <v>1268</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <v>18318</v>
+      </c>
+      <c r="E134">
+        <v>1269</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <v>18418</v>
+      </c>
+      <c r="E135">
+        <v>1274</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <v>18519</v>
+      </c>
+      <c r="E136">
+        <v>1278</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <v>18619</v>
+      </c>
+      <c r="E137">
+        <v>1280</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <v>18719</v>
+      </c>
+      <c r="E138">
+        <v>1283</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <v>18820</v>
+      </c>
+      <c r="E139">
+        <v>1284</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <v>18920</v>
+      </c>
+      <c r="E140">
+        <v>1286</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G140">
+        <f>SUM(F90:F140)/51</f>
+        <v>3.6862745098039214</v>
+      </c>
+    </row>
+    <row r="141" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <v>19021</v>
+      </c>
+      <c r="E141">
+        <v>1288</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <v>19122</v>
+      </c>
+      <c r="E142">
+        <v>1291</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <v>19222</v>
+      </c>
+      <c r="E143">
+        <v>1294</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <v>19323</v>
+      </c>
+      <c r="E144">
+        <v>1297</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <v>19424</v>
+      </c>
+      <c r="E145">
+        <v>1300</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <v>19524</v>
+      </c>
+      <c r="E146">
+        <v>1301</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <v>19624</v>
+      </c>
+      <c r="E147">
+        <v>1302</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D148">
+        <v>19724</v>
+      </c>
+      <c r="E148">
+        <v>1305</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D149">
+        <v>19824</v>
+      </c>
+      <c r="E149">
+        <v>1308</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D150">
+        <v>19924</v>
+      </c>
+      <c r="E150">
+        <v>1311</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D151">
+        <v>20024</v>
+      </c>
+      <c r="E151">
+        <v>1314</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D152">
+        <v>20125</v>
+      </c>
+      <c r="E152">
+        <v>1316</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D153">
+        <v>20226</v>
+      </c>
+      <c r="E153">
+        <v>1319</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D154">
+        <v>20326</v>
+      </c>
+      <c r="E154">
+        <v>1322</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D155">
+        <v>20426</v>
+      </c>
+      <c r="E155">
+        <v>1326</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D156">
+        <v>20526</v>
+      </c>
+      <c r="E156">
+        <v>1329</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D157">
+        <v>20626</v>
+      </c>
+      <c r="E157">
+        <v>1331</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D158">
+        <v>20727</v>
+      </c>
+      <c r="E158">
+        <v>1334</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D159">
+        <v>20827</v>
+      </c>
+      <c r="E159">
+        <v>1336</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D160">
+        <v>20928</v>
+      </c>
+      <c r="E160">
+        <v>1337</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D161">
+        <v>21028</v>
+      </c>
+      <c r="E161">
+        <v>1341</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D162">
+        <v>21129</v>
+      </c>
+      <c r="E162">
+        <v>1341</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D163">
+        <v>21229</v>
+      </c>
+      <c r="E163">
+        <v>1344</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D164">
+        <v>21329</v>
+      </c>
+      <c r="E164">
+        <v>1347</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D165">
+        <v>21429</v>
+      </c>
+      <c r="E165">
+        <v>1350</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>21529</v>
+      </c>
+      <c r="E166">
+        <v>1351</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D167">
+        <v>21630</v>
+      </c>
+      <c r="E167">
+        <v>1359</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D168">
+        <v>21731</v>
+      </c>
+      <c r="E168">
+        <v>1362</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D169">
+        <v>21831</v>
+      </c>
+      <c r="E169">
+        <v>1364</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D170">
+        <v>21931</v>
+      </c>
+      <c r="E170">
+        <v>1365</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D171">
+        <v>22032</v>
+      </c>
+      <c r="E171">
+        <v>1370</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D172">
+        <v>22133</v>
+      </c>
+      <c r="E172">
+        <v>1376</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D173">
+        <v>22233</v>
+      </c>
+      <c r="E173">
+        <v>1379</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D174">
+        <v>22333</v>
+      </c>
+      <c r="E174">
+        <v>1383</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D175">
+        <v>22433</v>
+      </c>
+      <c r="E175">
+        <v>1384</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D176">
+        <v>22533</v>
+      </c>
+      <c r="E176">
+        <v>1389</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D177">
+        <v>22633</v>
+      </c>
+      <c r="E177">
+        <v>1393</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D178">
+        <v>22734</v>
+      </c>
+      <c r="E178">
+        <v>1396</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D179">
+        <v>22834</v>
+      </c>
+      <c r="E179">
+        <v>1399</v>
+      </c>
+      <c r="F179">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D180">
+        <v>22935</v>
+      </c>
+      <c r="E180">
+        <v>1404</v>
+      </c>
+      <c r="F180">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D181">
+        <v>23035</v>
+      </c>
+      <c r="E181">
+        <v>1412</v>
+      </c>
+      <c r="F181">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D182">
+        <v>23136</v>
+      </c>
+      <c r="E182">
+        <v>1413</v>
+      </c>
+      <c r="F182">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D183">
+        <v>23237</v>
+      </c>
+      <c r="E183">
+        <v>1413</v>
+      </c>
+      <c r="F183">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D184">
+        <v>23337</v>
+      </c>
+      <c r="E184">
+        <v>1415</v>
+      </c>
+      <c r="F184">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D185">
+        <v>23437</v>
+      </c>
+      <c r="E185">
+        <v>1418</v>
+      </c>
+      <c r="F185">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D186">
+        <v>23537</v>
+      </c>
+      <c r="E186">
+        <v>1422</v>
+      </c>
+      <c r="F186">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D187">
+        <v>23638</v>
+      </c>
+      <c r="E187">
+        <v>1424</v>
+      </c>
+      <c r="F187">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D188">
+        <v>23739</v>
+      </c>
+      <c r="E188">
+        <v>1426</v>
+      </c>
+      <c r="F188">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D189">
+        <v>23840</v>
+      </c>
+      <c r="E189">
+        <v>1430</v>
+      </c>
+      <c r="F189">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D190">
+        <v>23940</v>
+      </c>
+      <c r="E190">
+        <v>1433</v>
+      </c>
+      <c r="F190">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D191">
+        <v>24040</v>
+      </c>
+      <c r="E191">
+        <v>1436</v>
+      </c>
+      <c r="F191">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D192">
+        <v>24140</v>
+      </c>
+      <c r="E192">
+        <v>1437</v>
+      </c>
+      <c r="F192">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D193">
+        <v>24240</v>
+      </c>
+      <c r="E193">
+        <v>1437</v>
+      </c>
+      <c r="F193">
+        <f>E193-E192</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D194">
+        <v>24340</v>
+      </c>
+      <c r="E194">
+        <v>1439</v>
+      </c>
+      <c r="F194">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D195">
+        <v>24441</v>
+      </c>
+      <c r="E195">
+        <v>1439</v>
+      </c>
+      <c r="F195">
+        <f t="shared" ref="F195:F258" si="3">E195-E194</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D196">
+        <v>24541</v>
+      </c>
+      <c r="E196">
+        <v>1443</v>
+      </c>
+      <c r="F196">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G196">
+        <f>SUM(F141:F196)/56</f>
+        <v>2.8035714285714284</v>
+      </c>
+    </row>
+    <row r="197" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D197">
+        <v>24642</v>
+      </c>
+      <c r="E197">
+        <v>1445</v>
+      </c>
+      <c r="F197">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D198">
+        <v>24743</v>
+      </c>
+      <c r="E198">
+        <v>1451</v>
+      </c>
+      <c r="F198">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D199">
+        <v>24843</v>
+      </c>
+      <c r="E199">
+        <v>1453</v>
+      </c>
+      <c r="F199">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D200">
+        <v>24943</v>
+      </c>
+      <c r="E200">
+        <v>1455</v>
+      </c>
+      <c r="F200">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D201">
+        <v>25043</v>
+      </c>
+      <c r="E201">
+        <v>1457</v>
+      </c>
+      <c r="F201">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D202">
+        <v>25143</v>
+      </c>
+      <c r="E202">
+        <v>1459</v>
+      </c>
+      <c r="F202">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D203">
+        <v>25243</v>
+      </c>
+      <c r="E203">
+        <v>1460</v>
+      </c>
+      <c r="F203">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D204">
+        <v>25343</v>
+      </c>
+      <c r="E204">
+        <v>1464</v>
+      </c>
+      <c r="F204">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D205">
+        <v>25444</v>
+      </c>
+      <c r="E205">
+        <v>1465</v>
+      </c>
+      <c r="F205">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D206">
+        <v>25544</v>
+      </c>
+      <c r="E206">
+        <v>1466</v>
+      </c>
+      <c r="F206">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D207">
+        <v>25644</v>
+      </c>
+      <c r="E207">
+        <v>1472</v>
+      </c>
+      <c r="F207">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D208">
+        <v>25744</v>
+      </c>
+      <c r="E208">
+        <v>1475</v>
+      </c>
+      <c r="F208">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D209">
+        <v>25844</v>
+      </c>
+      <c r="E209">
+        <v>1476</v>
+      </c>
+      <c r="F209">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D210">
+        <v>25945</v>
+      </c>
+      <c r="E210">
+        <v>1478</v>
+      </c>
+      <c r="F210">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D211">
+        <v>26045</v>
+      </c>
+      <c r="E211">
+        <v>1481</v>
+      </c>
+      <c r="F211">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D212">
+        <v>26145</v>
+      </c>
+      <c r="E212">
+        <v>1482</v>
+      </c>
+      <c r="F212">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D213">
+        <v>26245</v>
+      </c>
+      <c r="E213">
+        <v>1484</v>
+      </c>
+      <c r="F213">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D214">
+        <v>26345</v>
+      </c>
+      <c r="E214">
+        <v>1488</v>
+      </c>
+      <c r="F214">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D215">
+        <v>26446</v>
+      </c>
+      <c r="E215">
+        <v>1492</v>
+      </c>
+      <c r="F215">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D216">
+        <v>26546</v>
+      </c>
+      <c r="E216">
+        <v>1495</v>
+      </c>
+      <c r="F216">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D217">
+        <v>26646</v>
+      </c>
+      <c r="E217">
+        <v>1498</v>
+      </c>
+      <c r="F217">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D218">
+        <v>26746</v>
+      </c>
+      <c r="E218">
+        <v>1501</v>
+      </c>
+      <c r="F218">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D219">
+        <v>26847</v>
+      </c>
+      <c r="E219">
+        <v>1503</v>
+      </c>
+      <c r="F219">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D220">
+        <v>26948</v>
+      </c>
+      <c r="E220">
+        <v>1506</v>
+      </c>
+      <c r="F220">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D221">
+        <v>27048</v>
+      </c>
+      <c r="E221">
+        <v>1509</v>
+      </c>
+      <c r="F221">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D222">
+        <v>27149</v>
+      </c>
+      <c r="E222">
+        <v>1509</v>
+      </c>
+      <c r="F222">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D223">
+        <v>27250</v>
+      </c>
+      <c r="E223">
+        <v>1511</v>
+      </c>
+      <c r="F223">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D224">
+        <v>27350</v>
+      </c>
+      <c r="E224">
+        <v>1513</v>
+      </c>
+      <c r="F224">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D225">
+        <v>27451</v>
+      </c>
+      <c r="E225">
+        <v>1517</v>
+      </c>
+      <c r="F225">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D226">
+        <v>27551</v>
+      </c>
+      <c r="E226">
+        <v>1517</v>
+      </c>
+      <c r="F226">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G226">
+        <f>SUM(F197:F226)/30</f>
+        <v>2.4666666666666668</v>
+      </c>
+    </row>
+    <row r="227" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D227">
+        <v>29522</v>
+      </c>
+      <c r="E227">
+        <v>1559</v>
+      </c>
+      <c r="F227">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="228" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D228">
+        <v>29622</v>
+      </c>
+      <c r="E228">
+        <v>1560</v>
+      </c>
+      <c r="F228">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D229">
+        <v>29722</v>
+      </c>
+      <c r="E229">
+        <v>1561</v>
+      </c>
+      <c r="F229">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D230">
+        <v>29822</v>
+      </c>
+      <c r="E230">
+        <v>1562</v>
+      </c>
+      <c r="F230">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D231">
+        <v>29923</v>
+      </c>
+      <c r="E231">
+        <v>1562</v>
+      </c>
+      <c r="F231">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D232">
+        <v>30023</v>
+      </c>
+      <c r="E232">
+        <v>1565</v>
+      </c>
+      <c r="F232">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D233">
+        <v>30123</v>
+      </c>
+      <c r="E233">
+        <v>1567</v>
+      </c>
+      <c r="F233">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D234">
+        <v>30223</v>
+      </c>
+      <c r="E234">
+        <v>1571</v>
+      </c>
+      <c r="F234">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D235">
+        <v>30324</v>
+      </c>
+      <c r="E235">
+        <v>1576</v>
+      </c>
+      <c r="F235">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D236">
+        <v>30425</v>
+      </c>
+      <c r="E236">
+        <v>1578</v>
+      </c>
+      <c r="F236">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D237">
+        <v>30525</v>
+      </c>
+      <c r="E237">
+        <v>1580</v>
+      </c>
+      <c r="F237">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D238">
+        <v>30625</v>
+      </c>
+      <c r="E238">
+        <v>1581</v>
+      </c>
+      <c r="F238">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D239">
+        <v>30725</v>
+      </c>
+      <c r="E239">
+        <v>1583</v>
+      </c>
+      <c r="F239">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D240">
+        <v>30825</v>
+      </c>
+      <c r="E240">
+        <v>1584</v>
+      </c>
+      <c r="F240">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D241">
+        <v>30925</v>
+      </c>
+      <c r="E241">
+        <v>1584</v>
+      </c>
+      <c r="F241">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D242">
+        <v>31025</v>
+      </c>
+      <c r="E242">
+        <v>1586</v>
+      </c>
+      <c r="F242">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D243">
+        <v>31125</v>
+      </c>
+      <c r="E243">
+        <v>1589</v>
+      </c>
+      <c r="F243">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D244">
+        <v>31225</v>
+      </c>
+      <c r="E244">
+        <v>1591</v>
+      </c>
+      <c r="F244">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D245">
+        <v>31325</v>
+      </c>
+      <c r="E245">
+        <v>1595</v>
+      </c>
+      <c r="F245">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D246">
+        <v>31425</v>
+      </c>
+      <c r="E246">
+        <v>1596</v>
+      </c>
+      <c r="F246">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D247">
+        <v>31525</v>
+      </c>
+      <c r="E247">
+        <v>1597</v>
+      </c>
+      <c r="F247">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D248">
+        <v>31625</v>
+      </c>
+      <c r="E248">
+        <v>1599</v>
+      </c>
+      <c r="F248">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D249">
+        <v>31725</v>
+      </c>
+      <c r="E249">
+        <v>1601</v>
+      </c>
+      <c r="F249">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D250">
+        <v>31825</v>
+      </c>
+      <c r="E250">
+        <v>1603</v>
+      </c>
+      <c r="F250">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D251">
+        <v>31925</v>
+      </c>
+      <c r="E251">
+        <v>1605</v>
+      </c>
+      <c r="F251">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D252">
+        <v>32025</v>
+      </c>
+      <c r="E252">
+        <v>1606</v>
+      </c>
+      <c r="F252">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D253">
+        <v>32125</v>
+      </c>
+      <c r="E253">
+        <v>1609</v>
+      </c>
+      <c r="F253">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D254">
+        <v>32225</v>
+      </c>
+      <c r="E254">
+        <v>1611</v>
+      </c>
+      <c r="F254">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D255">
+        <v>32326</v>
+      </c>
+      <c r="E255">
+        <v>1613</v>
+      </c>
+      <c r="F255">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D256">
+        <v>32427</v>
+      </c>
+      <c r="E256">
+        <v>1615</v>
+      </c>
+      <c r="F256">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D257">
+        <v>32528</v>
+      </c>
+      <c r="E257">
+        <v>1618</v>
+      </c>
+      <c r="F257">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D258">
+        <v>32628</v>
+      </c>
+      <c r="E258">
+        <v>1622</v>
+      </c>
+      <c r="F258">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D259">
+        <v>32728</v>
+      </c>
+      <c r="E259">
+        <v>1624</v>
+      </c>
+      <c r="F259">
+        <f t="shared" ref="F259:F284" si="4">E259-E258</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D260">
+        <v>32828</v>
+      </c>
+      <c r="E260">
+        <v>1627</v>
+      </c>
+      <c r="F260">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D261">
+        <v>32929</v>
+      </c>
+      <c r="E261">
+        <v>1631</v>
+      </c>
+      <c r="F261">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D262">
+        <v>33029</v>
+      </c>
+      <c r="E262">
+        <v>1632</v>
+      </c>
+      <c r="F262">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D263">
+        <v>33129</v>
+      </c>
+      <c r="E263">
+        <v>1635</v>
+      </c>
+      <c r="F263">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D264">
+        <v>33229</v>
+      </c>
+      <c r="E264">
+        <v>1638</v>
+      </c>
+      <c r="F264">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D265">
+        <v>33330</v>
+      </c>
+      <c r="E265">
+        <v>1639</v>
+      </c>
+      <c r="F265">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G265">
+        <f>SUM(F228:F265)/38</f>
+        <v>2.1052631578947367</v>
+      </c>
+    </row>
+    <row r="266" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D266">
+        <v>33430</v>
+      </c>
+      <c r="E266">
+        <v>1639</v>
+      </c>
+      <c r="F266">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D267">
+        <v>33530</v>
+      </c>
+      <c r="E267">
+        <v>1642</v>
+      </c>
+      <c r="F267">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D268">
+        <v>33630</v>
+      </c>
+      <c r="E268">
+        <v>1645</v>
+      </c>
+      <c r="F268">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D269">
+        <v>33731</v>
+      </c>
+      <c r="E269">
+        <v>1648</v>
+      </c>
+      <c r="F269">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D270">
+        <v>33832</v>
+      </c>
+      <c r="E270">
+        <v>1650</v>
+      </c>
+      <c r="F270">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D271">
+        <v>33923</v>
+      </c>
+      <c r="E271">
+        <v>1652</v>
+      </c>
+      <c r="F271">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D272">
+        <v>34032</v>
+      </c>
+      <c r="E272">
+        <v>1656</v>
+      </c>
+      <c r="F272">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D273">
+        <v>34132</v>
+      </c>
+      <c r="E273">
+        <v>1656</v>
+      </c>
+      <c r="F273">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D274">
+        <v>34232</v>
+      </c>
+      <c r="E274">
+        <v>1658</v>
+      </c>
+      <c r="F274">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D275">
+        <v>34332</v>
+      </c>
+      <c r="E275">
+        <v>1660</v>
+      </c>
+      <c r="F275">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D276">
+        <v>34432</v>
+      </c>
+      <c r="E276">
+        <v>1661</v>
+      </c>
+      <c r="F276">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D277">
+        <v>34532</v>
+      </c>
+      <c r="E277">
+        <v>1662</v>
+      </c>
+      <c r="F277">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D278">
+        <v>34632</v>
+      </c>
+      <c r="E278">
+        <v>1662</v>
+      </c>
+      <c r="F278">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D279">
+        <v>34731</v>
+      </c>
+      <c r="E279">
+        <v>1664</v>
+      </c>
+      <c r="F279">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D280">
+        <v>34832</v>
+      </c>
+      <c r="E280">
+        <v>1665</v>
+      </c>
+      <c r="F280">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D281">
+        <v>34932</v>
+      </c>
+      <c r="E281">
+        <v>1666</v>
+      </c>
+      <c r="F281">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D282">
+        <v>35032</v>
+      </c>
+      <c r="E282">
+        <v>1670</v>
+      </c>
+      <c r="F282">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D283">
+        <v>35132</v>
+      </c>
+      <c r="E283">
+        <v>1674</v>
+      </c>
+      <c r="F283">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D284">
+        <v>35232</v>
+      </c>
+      <c r="E284">
+        <v>1676</v>
+      </c>
+      <c r="F284">
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>